<commit_message>
T7A - com dados da aula
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D7BEC0-C9F3-44D0-95E4-89B964627585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C28A6E-7A88-472A-A46D-84C24F04F1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -271,6 +271,78 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$K$3:$K$22</c:f>
@@ -278,64 +350,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.4347826086956527E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.3054830287206267E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.3475935828877004E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.2070006035003019E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.4200542005420058E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.1376564277588168E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5.4644808743169397E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.0638297872340425E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>9.4250706880301613E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>8.8668203582195418E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,64 +389,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.3037809647979138E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.2631578947368418E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.199760047990402E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5.1679586563307491E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.1293054771315642E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5.2631578947368418E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.0526315789473684E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5.181347150259067E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>5.5096418732782371E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>5.6657223796034002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -687,6 +699,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>112.78</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -696,6 +738,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>102.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>106.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>130.94999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2382,7 +2454,7 @@
   <dimension ref="A2:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2431,272 +2503,352 @@
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="e">
+      <c r="B3" s="2">
+        <v>95.6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>76.7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.15</v>
+      </c>
+      <c r="G3" s="1">
         <f>F3/E3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" s="1" t="e">
+        <v>3.9782608695652177</v>
+      </c>
+      <c r="H3" s="1">
         <f>(D3*C3)/B3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I3" s="1" t="e">
+        <v>14.762343096234311</v>
+      </c>
+      <c r="I3" s="1">
         <f>C3-((C3^2)/B3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J3" s="1" t="e">
+        <v>14.858577405857739</v>
+      </c>
+      <c r="J3" s="1">
         <f>D3-((D3^2)/B3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K3" s="1" t="e">
-        <f>1/C3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L3" s="1" t="e">
-        <f>1/D3</f>
-        <v>#DIV/0!</v>
+        <v>15.163493723849371</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K22" si="0">1/C3</f>
+        <v>5.4347826086956527E-2</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L22" si="1">1/D3</f>
+        <v>1.3037809647979138E-2</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="e">
-        <f t="shared" ref="G4:G22" si="0">F4/E4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" s="1" t="e">
-        <f t="shared" ref="H4:H22" si="1">(D4*C4)/B4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="1" t="e">
-        <f t="shared" ref="I4:I22" si="2">C4-((C4^2)/B4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J4" s="1" t="e">
-        <f t="shared" ref="J4:J22" si="3">D4-((D4^2)/B4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" s="1" t="e">
-        <f>1/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" s="1" t="e">
-        <f>1/D4</f>
-        <v>#DIV/0!</v>
+      <c r="B4" s="2">
+        <v>95.75</v>
+      </c>
+      <c r="C4" s="1">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="D4" s="1">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G22" si="2">F4/E4</f>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H22" si="3">(D4*C4)/B4</f>
+        <v>15.2</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I22" si="4">C4-((C4^2)/B4)</f>
+        <v>15.32</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J22" si="5">D4-((D4^2)/B4)</f>
+        <v>15.229765013054831</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3054830287206267E-2</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="e">
+      <c r="B5" s="2">
+        <v>102.1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>83.35</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="2"/>
+        <v>3.6956521739130439</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="3"/>
+        <v>15.265866797257589</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="4"/>
+        <v>15.275024485798236</v>
+      </c>
+      <c r="J5" s="1">
+        <f>D5-((D5^2)/B5)</f>
+        <v>15.306684622918709</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="1" t="e">
+        <v>5.3475935828877004E-2</v>
+      </c>
+      <c r="L5" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" s="1" t="e">
-        <f>1/C5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="1" t="e">
-        <f>1/D5</f>
-        <v>#DIV/0!</v>
+        <v>1.199760047990402E-2</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="e">
+      <c r="B6" s="2">
+        <v>102.15</v>
+      </c>
+      <c r="C6" s="1">
+        <v>82.85</v>
+      </c>
+      <c r="D6" s="1">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="3"/>
+        <v>15.694052863436124</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="4"/>
+        <v>15.653499755261876</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="5"/>
+        <v>15.684581497797357</v>
+      </c>
+      <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="1" t="e">
+        <v>1.2070006035003019E-2</v>
+      </c>
+      <c r="L6" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K6" s="1" t="e">
-        <f>1/C6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="1" t="e">
-        <f>1/D6</f>
-        <v>#DIV/0!</v>
+        <v>5.1679586563307491E-2</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="e">
+      <c r="B7" s="2">
+        <v>106.9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>18.45</v>
+      </c>
+      <c r="D7" s="1">
+        <v>88.55</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>3.804347826086957</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="3"/>
+        <v>15.282951356407857</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="4"/>
+        <v>15.265692235734331</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="5"/>
+        <v>15.200116931711889</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="1" t="e">
+        <v>5.4200542005420058E-2</v>
+      </c>
+      <c r="L7" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="1" t="e">
-        <f>1/C7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="1" t="e">
-        <f>1/D7</f>
-        <v>#DIV/0!</v>
+        <v>1.1293054771315642E-2</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="e">
+      <c r="B8" s="2">
+        <v>106.9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>87.9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="3"/>
+        <v>15.623012160898035</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="4"/>
+        <v>15.623012160898043</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="5"/>
+        <v>15.623012160898035</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="1" t="e">
+        <v>1.1376564277588168E-2</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="1" t="e">
-        <f>1/C8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="1" t="e">
-        <f>1/D8</f>
-        <v>#DIV/0!</v>
+        <v>5.2631578947368418E-2</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="e">
+      <c r="B9" s="2">
+        <v>113.1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>95</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F9" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1304347826086962</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="3"/>
+        <v>15.37135278514589</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="4"/>
+        <v>15.338992042440319</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="5"/>
+        <v>15.203359858532266</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="1" t="e">
+        <v>5.4644808743169397E-2</v>
+      </c>
+      <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="1" t="e">
-        <f>1/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L9" s="1" t="e">
-        <f>1/D9</f>
-        <v>#DIV/0!</v>
+        <v>1.0526315789473684E-2</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="e">
+      <c r="B10" s="2">
+        <v>113.05</v>
+      </c>
+      <c r="C10" s="1">
+        <v>94</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19.3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.19565217391304349</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="3"/>
+        <v>16.047766475011059</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="4"/>
+        <v>15.839893852277754</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="5"/>
+        <v>16.005086245024327</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="1" t="e">
+        <v>1.0638297872340425E-2</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="1" t="e">
-        <f>1/C10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="1" t="e">
-        <f>1/D10</f>
-        <v>#DIV/0!</v>
+        <v>5.181347150259067E-2</v>
       </c>
       <c r="W10" t="s">
         <v>11</v>
@@ -2706,68 +2858,88 @@
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="e">
+      <c r="B11" s="2">
+        <v>124.3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>106.1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17391304347826089</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="3"/>
+        <v>15.492477876106193</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="4"/>
+        <v>15.535156878519714</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="5"/>
+        <v>15.499778761061947</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="1" t="e">
+        <v>9.4250706880301613E-3</v>
+      </c>
+      <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="1" t="e">
-        <f>1/C11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11" s="1" t="e">
-        <f>1/D11</f>
-        <v>#DIV/0!</v>
+        <v>5.5096418732782371E-2</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="e">
+      <c r="B12" s="2">
+        <v>130.94999999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>112.78</v>
+      </c>
+      <c r="D12" s="1">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17391304347826089</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="3"/>
+        <v>15.200969835815195</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="4"/>
+        <v>15.648817105765545</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="5"/>
+        <v>15.271057655593737</v>
+      </c>
+      <c r="K12" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="1" t="e">
+        <v>8.8668203582195418E-3</v>
+      </c>
+      <c r="L12" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K12" s="1" t="e">
-        <f>1/C12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" s="1" t="e">
-        <f>1/D12</f>
-        <v>#DIV/0!</v>
+        <v>5.6657223796034002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
@@ -2780,29 +2952,23 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H13" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I13" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J13" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K13" s="1" t="e">
-        <f>1/C13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L13" s="1" t="e">
-        <f>1/D13</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -2814,29 +2980,23 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H14" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J14" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="1" t="e">
-        <f>1/C14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" s="1" t="e">
-        <f>1/D14</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -2848,29 +3008,23 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H15" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I15" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J15" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="1" t="e">
-        <f>1/C15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="1" t="e">
-        <f>1/D15</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -2882,29 +3036,23 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H16" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J16" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="1" t="e">
-        <f>1/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="1" t="e">
-        <f>1/D16</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
@@ -2916,29 +3064,23 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H17" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J17" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="1" t="e">
-        <f>1/C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L17" s="1" t="e">
-        <f>1/D17</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -2950,29 +3092,23 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H18" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J18" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="1" t="e">
-        <f>1/C18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="1" t="e">
-        <f>1/D18</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
@@ -2984,29 +3120,23 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H19" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I19" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J19" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K19" s="1" t="e">
-        <f>1/C19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L19" s="1" t="e">
-        <f>1/D19</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -3018,29 +3148,23 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H20" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J20" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="1" t="e">
-        <f>1/C20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="1" t="e">
-        <f>1/D20</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
@@ -3052,29 +3176,23 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H21" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I21" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J21" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="1" t="e">
-        <f>1/C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="1" t="e">
-        <f>1/D21</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -3086,29 +3204,23 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H22" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J22" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="1" t="e">
-        <f>1/C22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="1" t="e">
-        <f>1/D22</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3117,6 +3229,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A6AC9AE00E36404AA0D09428E6D89785" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="90a733a5ab80369601faf008bc080d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c5de1c3e-7813-4da7-ba52-5366b85aaf02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b20cf44b89237f95aaad323f9088c9f4" ns3:_="">
     <xsd:import namespace="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
@@ -3262,22 +3389,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE32EF5C-8F83-4888-B6EF-0E9A1DA73572}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3293,28 +3429,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
T7A - corrigir A e B
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C28A6E-7A88-472A-A46D-84C24F04F1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98081AB8-4459-4C73-B619-7A929D9C9C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>D (cm)</t>
   </si>
@@ -70,9 +70,6 @@
     <t>1/SO</t>
   </si>
   <si>
-    <t>f=declive / D</t>
-  </si>
-  <si>
     <t>2h (cm)</t>
   </si>
   <si>
@@ -92,7 +89,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +99,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -147,6 +150,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -345,10 +352,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$22</c:f>
+              <c:f>Sheet1!$K$3:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.4347826086956527E-2</c:v>
                 </c:pt>
@@ -384,10 +391,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$22</c:f>
+              <c:f>Sheet1!$L$3:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.3037809647979138E-2</c:v>
                 </c:pt>
@@ -695,10 +702,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$22</c:f>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>18.399999999999999</c:v>
                 </c:pt>
@@ -734,10 +741,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$22</c:f>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>95.6</c:v>
                 </c:pt>
@@ -2451,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34871357-AA4E-4AD0-9D7D-AF7CAC853938}">
-  <dimension ref="A2:W22"/>
+  <dimension ref="A2:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2463,7 +2470,7 @@
     <col min="10" max="10" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -2475,10 +2482,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -2499,7 +2506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2535,15 +2542,15 @@
         <v>15.163493723849371</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K22" si="0">1/C3</f>
+        <f t="shared" ref="K3:K12" si="0">1/C3</f>
         <v>5.4347826086956527E-2</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L22" si="1">1/D3</f>
+        <f t="shared" ref="L3:L12" si="1">1/D3</f>
         <v>1.3037809647979138E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2587,7 +2594,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -2631,7 +2638,7 @@
         <v>1.199760047990402E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -2675,7 +2682,7 @@
         <v>5.1679586563307491E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2719,7 +2726,7 @@
         <v>1.1293054771315642E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2763,7 +2770,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -2807,7 +2814,7 @@
         <v>1.0526315789473684E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -2850,13 +2857,10 @@
         <f t="shared" si="1"/>
         <v>5.181347150259067E-2</v>
       </c>
-      <c r="W10" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>124.3</v>
@@ -2898,7 +2902,7 @@
         <v>5.5096418732782371E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -2942,285 +2946,143 @@
         <v>5.6657223796034002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3229,21 +3091,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A6AC9AE00E36404AA0D09428E6D89785" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="90a733a5ab80369601faf008bc080d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c5de1c3e-7813-4da7-ba52-5366b85aaf02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b20cf44b89237f95aaad323f9088c9f4" ns3:_="">
     <xsd:import namespace="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
@@ -3389,31 +3236,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE32EF5C-8F83-4888-B6EF-0E9A1DA73572}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3429,4 +3267,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
T7A - com mais info e assintotas
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98081AB8-4459-4C73-B619-7A929D9C9C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236CEAE8-37E3-4DA8-A6C3-84EE2B0AC578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>D (cm)</t>
-  </si>
-  <si>
-    <t>SO (cm)</t>
   </si>
   <si>
     <t>Si (cm)</t>
@@ -75,12 +72,79 @@
   <si>
     <t>2h' (cm)</t>
   </si>
+  <si>
+    <t>Análise Estatística</t>
+  </si>
+  <si>
+    <t>u(m)</t>
+  </si>
+  <si>
+    <t>Declive (m)</t>
+  </si>
+  <si>
+    <t>Ordenada na origem (b)</t>
+  </si>
+  <si>
+    <t>u(b)</t>
+  </si>
+  <si>
+    <t>Interseção:</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Interseção de assíntota esquerda com y=0:</t>
+  </si>
+  <si>
+    <t>Interseção de assíntota direita com x=0:</t>
+  </si>
+  <si>
+    <t>Interseção da regressão com y=0:</t>
+  </si>
+  <si>
+    <t>Interseção da regressão com x=0:</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Lente +15</t>
+  </si>
+  <si>
+    <t>Lente +10</t>
+  </si>
+  <si>
+    <t>So (cm)</t>
+  </si>
+  <si>
+    <t>Máscara 2</t>
+  </si>
+  <si>
+    <t>Máscara 1</t>
+  </si>
+  <si>
+    <t>Sem máscara</t>
+  </si>
+  <si>
+    <t>1/SO (cm-1)</t>
+  </si>
+  <si>
+    <t>1/Si (cm-1)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,8 +152,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,12 +196,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -132,20 +230,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -153,8 +302,91 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,30 +584,30 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$12</c:f>
+              <c:f>Sheet1!$H$3:$H$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.4347826086956527E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5.3475935828877004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4200542005420058E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4644808743169397E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.3054830287206267E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3475935828877004E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>1.2070006035003019E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.4200542005420058E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.1376564277588168E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.4644808743169397E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0638297872340425E-2</c:v>
@@ -391,30 +623,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$12</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.3037809647979138E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.199760047990402E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1293054771315642E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0526315789473684E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5.2631578947368418E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.199760047990402E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>5.1679586563307491E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1293054771315642E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>5.2631578947368418E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0526315789473684E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5.181347150259067E-2</c:v>
@@ -467,7 +699,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>1/So (cm-1)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -529,7 +816,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>1/Si (cm-1)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -637,6 +979,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> em função de </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>S0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -710,22 +1085,22 @@
                   <c:v>18.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>76.599999999999994</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>82.85</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>18.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>87.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>94</c:v>
@@ -749,22 +1124,22 @@
                   <c:v>95.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>102.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>95.75</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>102.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>102.15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>106.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>106.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>113.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>113.05</c:v>
@@ -817,6 +1192,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>S0 (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -879,6 +1309,743 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>D</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414116351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> em função de </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>S0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>esquerda</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.25109405868314999"/>
+                  <c:y val="-7.345174335505307E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="6"/>
+            <c:backward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$C$3,Sheet1!$C$4,Sheet1!$C$5,Sheet1!$C$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$B$3,Sheet1!$B$4,Sheet1!$B$5,Sheet1!$B$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-DB36-44F4-8777-62931A273881}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>direita</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="10"/>
+            <c:backward val="75"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$C$7,Sheet1!$C$8,Sheet1!$C$9,Sheet1!$C$10,Sheet1!$C$11,Sheet1!$C$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>76.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$B$7,Sheet1!$B$8,Sheet1!$B$9,Sheet1!$B$10,Sheet1!$B$11,Sheet1!$B$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>95.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130.94999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-DB36-44F4-8777-62931A273881}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="414116351"/>
+        <c:axId val="414115519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="414116351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>S0 (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414115519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="414115519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>D</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1052,6 +2219,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1569,6 +2776,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2089,15 +3812,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:colOff>608606</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>994</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:colOff>303806</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>994</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2153,6 +3876,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289559</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>176605</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>392205</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>176605</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACFBFDE-36BA-4493-82BE-6F2D587C3E0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2458,639 +4219,1122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34871357-AA4E-4AD0-9D7D-AF7CAC853938}">
-  <dimension ref="A2:L22"/>
+  <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
     <col min="9" max="9" width="11.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="B3" s="9">
         <v>95.6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>18.399999999999999</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="9">
         <v>76.7</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="9">
         <v>9.15</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="25">
         <f>F3/E3</f>
         <v>3.9782608695652177</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="25">
+        <f>1/C3</f>
+        <v>5.4347826086956527E-2</v>
+      </c>
+      <c r="I3" s="25">
+        <f>1/D3</f>
+        <v>1.3037809647979138E-2</v>
+      </c>
+      <c r="J3" s="25">
         <f>(D3*C3)/B3</f>
         <v>14.762343096234311</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="25">
         <f>C3-((C3^2)/B3)</f>
         <v>14.858577405857739</v>
       </c>
-      <c r="J3" s="1">
+      <c r="L3" s="25">
         <f>D3-((D3^2)/B3)</f>
         <v>15.163493723849371</v>
       </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K12" si="0">1/C3</f>
-        <v>5.4347826086956527E-2</v>
-      </c>
-      <c r="L3" s="1">
-        <f t="shared" ref="L3:L12" si="1">1/D3</f>
-        <v>1.3037809647979138E-2</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>102.1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>18.7</v>
+      </c>
+      <c r="D4" s="9">
+        <v>83.35</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F4" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" ref="G4:G9" si="0">F4/E4</f>
+        <v>3.6956521739130439</v>
+      </c>
+      <c r="H4" s="25">
+        <f>1/C4</f>
+        <v>5.3475935828877004E-2</v>
+      </c>
+      <c r="I4" s="25">
+        <f>1/D4</f>
+        <v>1.199760047990402E-2</v>
+      </c>
+      <c r="J4" s="25">
+        <f>(D4*C4)/B4</f>
+        <v>15.265866797257589</v>
+      </c>
+      <c r="K4" s="25">
+        <f>C4-((C4^2)/B4)</f>
+        <v>15.275024485798236</v>
+      </c>
+      <c r="L4" s="25">
+        <f>D4-((D4^2)/B4)</f>
+        <v>15.306684622918709</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9">
+        <v>106.9</v>
+      </c>
+      <c r="C5" s="9">
+        <v>18.45</v>
+      </c>
+      <c r="D5" s="9">
+        <v>88.55</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F5" s="9">
+        <v>8.75</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="0"/>
+        <v>3.804347826086957</v>
+      </c>
+      <c r="H5" s="25">
+        <f>1/C5</f>
+        <v>5.4200542005420058E-2</v>
+      </c>
+      <c r="I5" s="25">
+        <f>1/D5</f>
+        <v>1.1293054771315642E-2</v>
+      </c>
+      <c r="J5" s="25">
+        <f>(D5*C5)/B5</f>
+        <v>15.282951356407857</v>
+      </c>
+      <c r="K5" s="25">
+        <f>C5-((C5^2)/B5)</f>
+        <v>15.265692235734331</v>
+      </c>
+      <c r="L5" s="25">
+        <f>D5-((D5^2)/B5)</f>
+        <v>15.200116931711889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9">
+        <v>113.1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>18.3</v>
+      </c>
+      <c r="D6" s="9">
+        <v>95</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9.5</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="0"/>
+        <v>4.1304347826086962</v>
+      </c>
+      <c r="H6" s="25">
+        <f>1/C6</f>
+        <v>5.4644808743169397E-2</v>
+      </c>
+      <c r="I6" s="25">
+        <f>1/D6</f>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="J6" s="25">
+        <f>(D6*C6)/B6</f>
+        <v>15.37135278514589</v>
+      </c>
+      <c r="K6" s="25">
+        <f>C6-((C6^2)/B6)</f>
+        <v>15.338992042440319</v>
+      </c>
+      <c r="L6" s="25">
+        <f>D6-((D6^2)/B6)</f>
+        <v>15.203359858532266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
         <v>95.75</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C7" s="9">
         <v>76.599999999999994</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D7" s="9">
         <v>19</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E7" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F7" s="9">
         <v>0.6</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" ref="G4:G22" si="2">F4/E4</f>
+      <c r="G7" s="25">
+        <f t="shared" si="0"/>
         <v>0.2608695652173913</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:H22" si="3">(D4*C4)/B4</f>
+      <c r="H7" s="25">
+        <f>1/C7</f>
+        <v>1.3054830287206267E-2</v>
+      </c>
+      <c r="I7" s="25">
+        <f>1/D7</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="J7" s="25">
+        <f>(D7*C7)/B7</f>
         <v>15.2</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" ref="I4:I22" si="4">C4-((C4^2)/B4)</f>
+      <c r="K7" s="25">
+        <f>C7-((C7^2)/B7)</f>
         <v>15.32</v>
       </c>
-      <c r="J4" s="1">
-        <f t="shared" ref="J4:J22" si="5">D4-((D4^2)/B4)</f>
+      <c r="L7" s="25">
+        <f>D7-((D7^2)/B7)</f>
         <v>15.229765013054831</v>
       </c>
-      <c r="K4" s="1">
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>102.15</v>
+      </c>
+      <c r="C8" s="9">
+        <v>82.85</v>
+      </c>
+      <c r="D8" s="9">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
-        <v>1.3054830287206267E-2</v>
-      </c>
-      <c r="L4" s="1">
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="H8" s="25">
+        <f>1/C8</f>
+        <v>1.2070006035003019E-2</v>
+      </c>
+      <c r="I8" s="25">
+        <f>1/D8</f>
+        <v>5.1679586563307491E-2</v>
+      </c>
+      <c r="J8" s="25">
+        <f>(D8*C8)/B8</f>
+        <v>15.694052863436124</v>
+      </c>
+      <c r="K8" s="25">
+        <f>C8-((C8^2)/B8)</f>
+        <v>15.653499755261876</v>
+      </c>
+      <c r="L8" s="25">
+        <f>D8-((D8^2)/B8)</f>
+        <v>15.684581497797357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <v>106.9</v>
+      </c>
+      <c r="C9" s="9">
+        <v>87.9</v>
+      </c>
+      <c r="D9" s="9">
+        <v>19</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="25">
+        <f t="shared" si="0"/>
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="H9" s="25">
+        <f>1/C9</f>
+        <v>1.1376564277588168E-2</v>
+      </c>
+      <c r="I9" s="25">
+        <f>1/D9</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="J9" s="25">
+        <f>(D9*C9)/B9</f>
+        <v>15.623012160898035</v>
+      </c>
+      <c r="K9" s="25">
+        <f>C9-((C9^2)/B9)</f>
+        <v>15.623012160898043</v>
+      </c>
+      <c r="L9" s="25">
+        <f>D9-((D9^2)/B9)</f>
+        <v>15.623012160898035</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9">
+        <v>113.05</v>
+      </c>
+      <c r="C10" s="9">
+        <v>94</v>
+      </c>
+      <c r="D10" s="9">
+        <v>19.3</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="G10" s="25">
+        <f t="shared" ref="G10:G12" si="1">F10/E10</f>
+        <v>0.19565217391304349</v>
+      </c>
+      <c r="H10" s="25">
+        <f>1/C10</f>
+        <v>1.0638297872340425E-2</v>
+      </c>
+      <c r="I10" s="25">
+        <f>1/D10</f>
+        <v>5.181347150259067E-2</v>
+      </c>
+      <c r="J10" s="25">
+        <f>(D10*C10)/B10</f>
+        <v>16.047766475011059</v>
+      </c>
+      <c r="K10" s="25">
+        <f>C10-((C10^2)/B10)</f>
+        <v>15.839893852277754</v>
+      </c>
+      <c r="L10" s="25">
+        <f>D10-((D10^2)/B10)</f>
+        <v>16.005086245024327</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="12">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="12">
+        <f>1/ Y10</f>
+        <v>15.105740181268883</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9">
+        <v>124.3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>106.1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="G11" s="25">
         <f t="shared" si="1"/>
-        <v>5.2631578947368418E-2</v>
-      </c>
+        <v>0.17391304347826089</v>
+      </c>
+      <c r="H11" s="25">
+        <f>1/C11</f>
+        <v>9.4250706880301613E-3</v>
+      </c>
+      <c r="I11" s="25">
+        <f>1/D11</f>
+        <v>5.5096418732782371E-2</v>
+      </c>
+      <c r="J11" s="25">
+        <f>(D11*C11)/B11</f>
+        <v>15.492477876106193</v>
+      </c>
+      <c r="K11" s="25">
+        <f>C11-((C11^2)/B11)</f>
+        <v>15.535156878519714</v>
+      </c>
+      <c r="L11" s="25">
+        <f>D11-((D11^2)/B11)</f>
+        <v>15.499778761061947</v>
+      </c>
+      <c r="W11" s="15"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <v>102.1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>18.7</v>
-      </c>
-      <c r="D5" s="1">
-        <v>83.35</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="B12" s="9">
+        <v>130.94999999999999</v>
+      </c>
+      <c r="C12" s="9">
+        <v>112.78</v>
+      </c>
+      <c r="D12" s="9">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="E12" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F5" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="G5" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6956521739130439</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F12" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="25">
+        <f t="shared" si="1"/>
+        <v>0.17391304347826089</v>
+      </c>
+      <c r="H12" s="25">
+        <f>1/C12</f>
+        <v>8.8668203582195418E-3</v>
+      </c>
+      <c r="I12" s="25">
+        <f>1/D12</f>
+        <v>5.6657223796034002E-2</v>
+      </c>
+      <c r="J12" s="25">
+        <f>(D12*C12)/B12</f>
+        <v>15.200969835815195</v>
+      </c>
+      <c r="K12" s="25">
+        <f>C12-((C12^2)/B12)</f>
+        <v>15.648817105765545</v>
+      </c>
+      <c r="L12" s="25">
+        <f>D12-((D12^2)/B12)</f>
+        <v>15.271057655593737</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="AA12" s="12">
+        <f>1/Z12</f>
+        <v>15.649452269170579</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="24">
+        <f>AVERAGE(J3:J12)</f>
+        <v>15.394079324631225</v>
+      </c>
+      <c r="K13" s="24">
+        <f>AVERAGE(K3:K12)</f>
+        <v>15.435866592255355</v>
+      </c>
+      <c r="L13" s="24">
+        <f t="shared" ref="L13" si="2">AVERAGE(L3:L12)</f>
+        <v>15.418693647044245</v>
+      </c>
+      <c r="W13" s="15"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="22">
+        <f t="array" ref="C15:D16">LINEST(I3:I12,H3:H12,TRUE,TRUE)</f>
+        <v>-0.96409120532709625</v>
+      </c>
+      <c r="D15" s="22">
+        <v>6.393354451691699E-2</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="22">
+        <v>1.6959264966798147E-2</v>
+      </c>
+      <c r="D16" s="22">
+        <v>5.9871925775196099E-4</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="22" t="e">
+        <f t="array" ref="C19:D20">LINEST(I7:I16,H7:H16,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="32"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D20" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B23" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="22" t="e">
+        <f t="array" ref="C23:D24">LINEST(I11:I20,H11:H20,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D23" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D24" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="Y27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="11">
+        <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(B7:B12,C7:C12))/(SLOPE(B7:B12,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
+        <v>22.145526015082648</v>
+      </c>
+      <c r="D28" s="11">
+        <f>SLOPE(B7:B12,C7:C12)*C28+INTERCEPT(B7:B12,C7:C12)</f>
+        <v>43.323863375679785</v>
+      </c>
+      <c r="E28" s="7">
+        <v>11.073</v>
+      </c>
+      <c r="F28" s="7">
+        <v>10.831</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="23">
+        <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(Y19:Y24,C7:C12))/(SLOPE(Y19:Y24,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
+        <v>24.756981786643593</v>
+      </c>
+      <c r="D29" s="12">
+        <f>SLOPE(B3:B6,C3:C6)*C29+INTERCEPT(B3:B6,C3:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="23">
+        <f>C29</f>
+        <v>24.756981786643593</v>
+      </c>
+      <c r="F29" s="23"/>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="Y30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="12">
+        <v>0</v>
+      </c>
+      <c r="D31" s="12">
+        <v>21.914000000000001</v>
+      </c>
+      <c r="E31" s="12">
+        <f>D31</f>
+        <v>21.914000000000001</v>
+      </c>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="9">
+        <v>39.5</v>
+      </c>
+      <c r="C36" s="9">
+        <v>15</v>
+      </c>
+      <c r="D36" s="9">
+        <v>24.5</v>
+      </c>
+      <c r="E36" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F36" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="G36" s="25">
+        <f>F36/E36</f>
+        <v>1.6086956521739133</v>
+      </c>
+      <c r="H36" s="25">
+        <f>1/C36</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I36" s="25">
+        <f>1/D36</f>
+        <v>4.0816326530612242E-2</v>
+      </c>
+      <c r="J36" s="25">
+        <f>D36*C36/B36</f>
+        <v>9.3037974683544302</v>
+      </c>
+      <c r="K36" s="25">
+        <f>C36-C36^2/B36</f>
+        <v>9.3037974683544302</v>
+      </c>
+      <c r="L36" s="25">
+        <f>D36-D36^2/B36</f>
+        <v>9.3037974683544302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="9">
+        <v>43.9</v>
+      </c>
+      <c r="C37" s="9">
+        <v>15</v>
+      </c>
+      <c r="D37" s="9">
+        <v>28.9</v>
+      </c>
+      <c r="E37" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F37" s="9">
+        <v>4</v>
+      </c>
+      <c r="G37" s="25">
+        <f t="shared" ref="G37:G38" si="3">F37/E37</f>
+        <v>1.7391304347826089</v>
+      </c>
+      <c r="H37" s="25">
+        <f t="shared" ref="H37:H38" si="4">1/C37</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I37" s="25">
+        <f t="shared" ref="I37:I38" si="5">1/D37</f>
+        <v>3.4602076124567477E-2</v>
+      </c>
+      <c r="J37" s="25">
+        <f t="shared" ref="J37:J38" si="6">D37*C37/B37</f>
+        <v>9.8747152619589986</v>
+      </c>
+      <c r="K37" s="25">
+        <f t="shared" ref="K37:K38" si="7">C37-C37^2/B37</f>
+        <v>9.8747152619589968</v>
+      </c>
+      <c r="L37" s="25">
+        <f t="shared" ref="L37:L38" si="8">D37-D37^2/B37</f>
+        <v>9.8747152619589968</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="9">
+        <v>41.25</v>
+      </c>
+      <c r="C38" s="9">
+        <v>15</v>
+      </c>
+      <c r="D38" s="9">
+        <v>26.75</v>
+      </c>
+      <c r="E38" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F38" s="9">
+        <v>4.3</v>
+      </c>
+      <c r="G38" s="25">
         <f t="shared" si="3"/>
-        <v>15.265866797257589</v>
-      </c>
-      <c r="I5" s="1">
+        <v>1.8695652173913044</v>
+      </c>
+      <c r="H38" s="25">
         <f t="shared" si="4"/>
-        <v>15.275024485798236</v>
-      </c>
-      <c r="J5" s="1">
-        <f>D5-((D5^2)/B5)</f>
-        <v>15.306684622918709</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3475935828877004E-2</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" si="1"/>
-        <v>1.199760047990402E-2</v>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I38" s="25">
+        <f t="shared" si="5"/>
+        <v>3.7383177570093455E-2</v>
+      </c>
+      <c r="J38" s="25">
+        <f t="shared" si="6"/>
+        <v>9.7272727272727266</v>
+      </c>
+      <c r="K38" s="25">
+        <f t="shared" si="7"/>
+        <v>9.5454545454545467</v>
+      </c>
+      <c r="L38" s="25">
+        <f t="shared" si="8"/>
+        <v>9.4030303030303024</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>102.15</v>
-      </c>
-      <c r="C6" s="1">
-        <v>82.85</v>
-      </c>
-      <c r="D6" s="1">
-        <v>19.350000000000001</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="2"/>
-        <v>0.21739130434782611</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="3"/>
-        <v>15.694052863436124</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="4"/>
-        <v>15.653499755261876</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="5"/>
-        <v>15.684581497797357</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2070006035003019E-2</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="1"/>
-        <v>5.1679586563307491E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>106.9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>18.45</v>
-      </c>
-      <c r="D7" s="1">
-        <v>88.55</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F7" s="1">
-        <v>8.75</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="2"/>
-        <v>3.804347826086957</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="3"/>
-        <v>15.282951356407857</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="4"/>
-        <v>15.265692235734331</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="5"/>
-        <v>15.200116931711889</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>5.4200542005420058E-2</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1293054771315642E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>106.9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>87.9</v>
-      </c>
-      <c r="D8" s="1">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="2"/>
-        <v>0.21739130434782611</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="3"/>
-        <v>15.623012160898035</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="4"/>
-        <v>15.623012160898043</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="5"/>
-        <v>15.623012160898035</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1376564277588168E-2</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="1"/>
-        <v>5.2631578947368418E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>113.1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>18.3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>95</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F9" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="2"/>
-        <v>4.1304347826086962</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="3"/>
-        <v>15.37135278514589</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" si="4"/>
-        <v>15.338992042440319</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="5"/>
-        <v>15.203359858532266</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="0"/>
-        <v>5.4644808743169397E-2</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0526315789473684E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>113.05</v>
-      </c>
-      <c r="C10" s="1">
-        <v>94</v>
-      </c>
-      <c r="D10" s="1">
-        <v>19.3</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.19565217391304349</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="3"/>
-        <v>16.047766475011059</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="4"/>
-        <v>15.839893852277754</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="5"/>
-        <v>16.005086245024327</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0638297872340425E-2</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="1"/>
-        <v>5.181347150259067E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2">
-        <v>124.3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>106.1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>18.149999999999999</v>
-      </c>
-      <c r="E11" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.17391304347826089</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="3"/>
-        <v>15.492477876106193</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="4"/>
-        <v>15.535156878519714</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="5"/>
-        <v>15.499778761061947</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="0"/>
-        <v>9.4250706880301613E-3</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="1"/>
-        <v>5.5096418732782371E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2">
-        <v>130.94999999999999</v>
-      </c>
-      <c r="C12" s="1">
-        <v>112.78</v>
-      </c>
-      <c r="D12" s="1">
-        <v>17.649999999999999</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.17391304347826089</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="3"/>
-        <v>15.200969835815195</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="4"/>
-        <v>15.648817105765545</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="5"/>
-        <v>15.271057655593737</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="0"/>
-        <v>8.8668203582195418E-3</v>
-      </c>
-      <c r="L12" s="1">
-        <f t="shared" si="1"/>
-        <v>5.6657223796034002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="25">
+        <f>AVERAGE(J36:J38)</f>
+        <v>9.6352618191953852</v>
+      </c>
+      <c r="K39" s="25">
+        <f t="shared" ref="K39:L39" si="9">AVERAGE(K36:K38)</f>
+        <v>9.5746557585893246</v>
+      </c>
+      <c r="L39" s="25">
+        <f t="shared" si="9"/>
+        <v>9.5271810111145765</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <mergeCells count="30">
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AA12:AA13"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="E31:F32"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="W10:X11"/>
+    <mergeCell ref="W12:X13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Y12:Y13"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+  </mergeCells>
+  <pageMargins left="0.01" right="0.01" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A6AC9AE00E36404AA0D09428E6D89785" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="90a733a5ab80369601faf008bc080d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c5de1c3e-7813-4da7-ba52-5366b85aaf02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b20cf44b89237f95aaad323f9088c9f4" ns3:_="">
     <xsd:import namespace="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
@@ -3236,7 +5480,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3245,13 +5489,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE32EF5C-8F83-4888-B6EF-0E9A1DA73572}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3269,26 +5523,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
T7A - análise estatistica das 2 retas incluida
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236CEAE8-37E3-4DA8-A6C3-84EE2B0AC578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCE4159-77F4-41E4-A524-67E8503BBA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>D (cm)</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>1/Si (cm-1)</t>
+  </si>
+  <si>
+    <t>Reta da Esquerda</t>
+  </si>
+  <si>
+    <t>Reta da Direita</t>
   </si>
 </sst>
 </file>
@@ -324,45 +330,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,13 +355,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -387,6 +366,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4221,8 +4227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34871357-AA4E-4AD0-9D7D-AF7CAC853938}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4243,19 +4249,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -4312,28 +4318,28 @@
       <c r="F3" s="9">
         <v>9.15</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="15">
         <f>F3/E3</f>
         <v>3.9782608695652177</v>
       </c>
-      <c r="H3" s="25">
-        <f>1/C3</f>
+      <c r="H3" s="15">
+        <f t="shared" ref="H3:H12" si="0">1/C3</f>
         <v>5.4347826086956527E-2</v>
       </c>
-      <c r="I3" s="25">
-        <f>1/D3</f>
+      <c r="I3" s="15">
+        <f t="shared" ref="I3:I12" si="1">1/D3</f>
         <v>1.3037809647979138E-2</v>
       </c>
-      <c r="J3" s="25">
-        <f>(D3*C3)/B3</f>
+      <c r="J3" s="15">
+        <f t="shared" ref="J3:J12" si="2">(D3*C3)/B3</f>
         <v>14.762343096234311</v>
       </c>
-      <c r="K3" s="25">
-        <f>C3-((C3^2)/B3)</f>
+      <c r="K3" s="15">
+        <f t="shared" ref="K3:K12" si="3">C3-((C3^2)/B3)</f>
         <v>14.858577405857739</v>
       </c>
-      <c r="L3" s="25">
-        <f>D3-((D3^2)/B3)</f>
+      <c r="L3" s="15">
+        <f t="shared" ref="L3:L12" si="4">D3-((D3^2)/B3)</f>
         <v>15.163493723849371</v>
       </c>
     </row>
@@ -4356,28 +4362,28 @@
       <c r="F4" s="9">
         <v>8.5</v>
       </c>
-      <c r="G4" s="25">
-        <f t="shared" ref="G4:G9" si="0">F4/E4</f>
+      <c r="G4" s="15">
+        <f t="shared" ref="G4:G9" si="5">F4/E4</f>
         <v>3.6956521739130439</v>
       </c>
-      <c r="H4" s="25">
-        <f>1/C4</f>
+      <c r="H4" s="15">
+        <f t="shared" si="0"/>
         <v>5.3475935828877004E-2</v>
       </c>
-      <c r="I4" s="25">
-        <f>1/D4</f>
+      <c r="I4" s="15">
+        <f t="shared" si="1"/>
         <v>1.199760047990402E-2</v>
       </c>
-      <c r="J4" s="25">
-        <f>(D4*C4)/B4</f>
+      <c r="J4" s="15">
+        <f t="shared" si="2"/>
         <v>15.265866797257589</v>
       </c>
-      <c r="K4" s="25">
-        <f>C4-((C4^2)/B4)</f>
+      <c r="K4" s="15">
+        <f t="shared" si="3"/>
         <v>15.275024485798236</v>
       </c>
-      <c r="L4" s="25">
-        <f>D4-((D4^2)/B4)</f>
+      <c r="L4" s="15">
+        <f t="shared" si="4"/>
         <v>15.306684622918709</v>
       </c>
     </row>
@@ -4400,28 +4406,28 @@
       <c r="F5" s="9">
         <v>8.75</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="15">
+        <f t="shared" si="5"/>
+        <v>3.804347826086957</v>
+      </c>
+      <c r="H5" s="15">
         <f t="shared" si="0"/>
-        <v>3.804347826086957</v>
-      </c>
-      <c r="H5" s="25">
-        <f>1/C5</f>
         <v>5.4200542005420058E-2</v>
       </c>
-      <c r="I5" s="25">
-        <f>1/D5</f>
+      <c r="I5" s="15">
+        <f t="shared" si="1"/>
         <v>1.1293054771315642E-2</v>
       </c>
-      <c r="J5" s="25">
-        <f>(D5*C5)/B5</f>
+      <c r="J5" s="15">
+        <f t="shared" si="2"/>
         <v>15.282951356407857</v>
       </c>
-      <c r="K5" s="25">
-        <f>C5-((C5^2)/B5)</f>
+      <c r="K5" s="15">
+        <f t="shared" si="3"/>
         <v>15.265692235734331</v>
       </c>
-      <c r="L5" s="25">
-        <f>D5-((D5^2)/B5)</f>
+      <c r="L5" s="15">
+        <f t="shared" si="4"/>
         <v>15.200116931711889</v>
       </c>
     </row>
@@ -4444,28 +4450,28 @@
       <c r="F6" s="9">
         <v>9.5</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="15">
+        <f t="shared" si="5"/>
+        <v>4.1304347826086962</v>
+      </c>
+      <c r="H6" s="15">
         <f t="shared" si="0"/>
-        <v>4.1304347826086962</v>
-      </c>
-      <c r="H6" s="25">
-        <f>1/C6</f>
         <v>5.4644808743169397E-2</v>
       </c>
-      <c r="I6" s="25">
-        <f>1/D6</f>
+      <c r="I6" s="15">
+        <f t="shared" si="1"/>
         <v>1.0526315789473684E-2</v>
       </c>
-      <c r="J6" s="25">
-        <f>(D6*C6)/B6</f>
+      <c r="J6" s="15">
+        <f t="shared" si="2"/>
         <v>15.37135278514589</v>
       </c>
-      <c r="K6" s="25">
-        <f>C6-((C6^2)/B6)</f>
+      <c r="K6" s="15">
+        <f t="shared" si="3"/>
         <v>15.338992042440319</v>
       </c>
-      <c r="L6" s="25">
-        <f>D6-((D6^2)/B6)</f>
+      <c r="L6" s="15">
+        <f t="shared" si="4"/>
         <v>15.203359858532266</v>
       </c>
     </row>
@@ -4488,28 +4494,28 @@
       <c r="F7" s="9">
         <v>0.6</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="15">
+        <f t="shared" si="5"/>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="H7" s="15">
         <f t="shared" si="0"/>
-        <v>0.2608695652173913</v>
-      </c>
-      <c r="H7" s="25">
-        <f>1/C7</f>
         <v>1.3054830287206267E-2</v>
       </c>
-      <c r="I7" s="25">
-        <f>1/D7</f>
+      <c r="I7" s="15">
+        <f t="shared" si="1"/>
         <v>5.2631578947368418E-2</v>
       </c>
-      <c r="J7" s="25">
-        <f>(D7*C7)/B7</f>
+      <c r="J7" s="15">
+        <f t="shared" si="2"/>
         <v>15.2</v>
       </c>
-      <c r="K7" s="25">
-        <f>C7-((C7^2)/B7)</f>
+      <c r="K7" s="15">
+        <f t="shared" si="3"/>
         <v>15.32</v>
       </c>
-      <c r="L7" s="25">
-        <f>D7-((D7^2)/B7)</f>
+      <c r="L7" s="15">
+        <f t="shared" si="4"/>
         <v>15.229765013054831</v>
       </c>
     </row>
@@ -4532,28 +4538,28 @@
       <c r="F8" s="9">
         <v>0.5</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="15">
+        <f t="shared" si="5"/>
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="H8" s="15">
         <f t="shared" si="0"/>
-        <v>0.21739130434782611</v>
-      </c>
-      <c r="H8" s="25">
-        <f>1/C8</f>
         <v>1.2070006035003019E-2</v>
       </c>
-      <c r="I8" s="25">
-        <f>1/D8</f>
+      <c r="I8" s="15">
+        <f t="shared" si="1"/>
         <v>5.1679586563307491E-2</v>
       </c>
-      <c r="J8" s="25">
-        <f>(D8*C8)/B8</f>
+      <c r="J8" s="15">
+        <f t="shared" si="2"/>
         <v>15.694052863436124</v>
       </c>
-      <c r="K8" s="25">
-        <f>C8-((C8^2)/B8)</f>
+      <c r="K8" s="15">
+        <f t="shared" si="3"/>
         <v>15.653499755261876</v>
       </c>
-      <c r="L8" s="25">
-        <f>D8-((D8^2)/B8)</f>
+      <c r="L8" s="15">
+        <f t="shared" si="4"/>
         <v>15.684581497797357</v>
       </c>
     </row>
@@ -4576,28 +4582,28 @@
       <c r="F9" s="9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="15">
+        <f t="shared" si="5"/>
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="H9" s="15">
         <f t="shared" si="0"/>
-        <v>0.21739130434782611</v>
-      </c>
-      <c r="H9" s="25">
-        <f>1/C9</f>
         <v>1.1376564277588168E-2</v>
       </c>
-      <c r="I9" s="25">
-        <f>1/D9</f>
+      <c r="I9" s="15">
+        <f t="shared" si="1"/>
         <v>5.2631578947368418E-2</v>
       </c>
-      <c r="J9" s="25">
-        <f>(D9*C9)/B9</f>
+      <c r="J9" s="15">
+        <f t="shared" si="2"/>
         <v>15.623012160898035</v>
       </c>
-      <c r="K9" s="25">
-        <f>C9-((C9^2)/B9)</f>
+      <c r="K9" s="15">
+        <f t="shared" si="3"/>
         <v>15.623012160898043</v>
       </c>
-      <c r="L9" s="25">
-        <f>D9-((D9^2)/B9)</f>
+      <c r="L9" s="15">
+        <f t="shared" si="4"/>
         <v>15.623012160898035</v>
       </c>
       <c r="Y9" s="2" t="s">
@@ -4629,41 +4635,41 @@
       <c r="F10" s="9">
         <v>0.45</v>
       </c>
-      <c r="G10" s="25">
-        <f t="shared" ref="G10:G12" si="1">F10/E10</f>
+      <c r="G10" s="15">
+        <f t="shared" ref="G10:G12" si="6">F10/E10</f>
         <v>0.19565217391304349</v>
       </c>
-      <c r="H10" s="25">
-        <f>1/C10</f>
+      <c r="H10" s="15">
+        <f t="shared" si="0"/>
         <v>1.0638297872340425E-2</v>
       </c>
-      <c r="I10" s="25">
-        <f>1/D10</f>
+      <c r="I10" s="15">
+        <f t="shared" si="1"/>
         <v>5.181347150259067E-2</v>
       </c>
-      <c r="J10" s="25">
-        <f>(D10*C10)/B10</f>
+      <c r="J10" s="15">
+        <f t="shared" si="2"/>
         <v>16.047766475011059</v>
       </c>
-      <c r="K10" s="25">
-        <f>C10-((C10^2)/B10)</f>
+      <c r="K10" s="15">
+        <f t="shared" si="3"/>
         <v>15.839893852277754</v>
       </c>
-      <c r="L10" s="25">
-        <f>D10-((D10^2)/B10)</f>
+      <c r="L10" s="15">
+        <f t="shared" si="4"/>
         <v>16.005086245024327</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="W10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="12">
+      <c r="X10" s="31"/>
+      <c r="Y10" s="25">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="Z10" s="25">
         <v>0</v>
       </c>
-      <c r="AA10" s="12">
+      <c r="AA10" s="25">
         <f>1/ Y10</f>
         <v>15.105740181268883</v>
       </c>
@@ -4687,35 +4693,35 @@
       <c r="F11" s="9">
         <v>0.4</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="15">
+        <f t="shared" si="6"/>
+        <v>0.17391304347826089</v>
+      </c>
+      <c r="H11" s="15">
+        <f t="shared" si="0"/>
+        <v>9.4250706880301613E-3</v>
+      </c>
+      <c r="I11" s="15">
         <f t="shared" si="1"/>
-        <v>0.17391304347826089</v>
-      </c>
-      <c r="H11" s="25">
-        <f>1/C11</f>
-        <v>9.4250706880301613E-3</v>
-      </c>
-      <c r="I11" s="25">
-        <f>1/D11</f>
         <v>5.5096418732782371E-2</v>
       </c>
-      <c r="J11" s="25">
-        <f>(D11*C11)/B11</f>
+      <c r="J11" s="15">
+        <f t="shared" si="2"/>
         <v>15.492477876106193</v>
       </c>
-      <c r="K11" s="25">
-        <f>C11-((C11^2)/B11)</f>
+      <c r="K11" s="15">
+        <f t="shared" si="3"/>
         <v>15.535156878519714</v>
       </c>
-      <c r="L11" s="25">
-        <f>D11-((D11^2)/B11)</f>
+      <c r="L11" s="15">
+        <f t="shared" si="4"/>
         <v>15.499778761061947</v>
       </c>
-      <c r="W11" s="15"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -4736,41 +4742,41 @@
       <c r="F12" s="9">
         <v>0.4</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="15">
+        <f t="shared" si="6"/>
+        <v>0.17391304347826089</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="0"/>
+        <v>8.8668203582195418E-3</v>
+      </c>
+      <c r="I12" s="15">
         <f t="shared" si="1"/>
-        <v>0.17391304347826089</v>
-      </c>
-      <c r="H12" s="25">
-        <f>1/C12</f>
-        <v>8.8668203582195418E-3</v>
-      </c>
-      <c r="I12" s="25">
-        <f>1/D12</f>
         <v>5.6657223796034002E-2</v>
       </c>
-      <c r="J12" s="25">
-        <f>(D12*C12)/B12</f>
+      <c r="J12" s="15">
+        <f t="shared" si="2"/>
         <v>15.200969835815195</v>
       </c>
-      <c r="K12" s="25">
-        <f>C12-((C12^2)/B12)</f>
+      <c r="K12" s="15">
+        <f t="shared" si="3"/>
         <v>15.648817105765545</v>
       </c>
-      <c r="L12" s="25">
-        <f>D12-((D12^2)/B12)</f>
+      <c r="L12" s="15">
+        <f t="shared" si="4"/>
         <v>15.271057655593737</v>
       </c>
-      <c r="W12" s="15" t="s">
+      <c r="W12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="12">
+      <c r="X12" s="31"/>
+      <c r="Y12" s="25">
         <v>0</v>
       </c>
-      <c r="Z12" s="12">
+      <c r="Z12" s="25">
         <v>6.3899999999999998E-2</v>
       </c>
-      <c r="AA12" s="12">
+      <c r="AA12" s="25">
         <f>1/Z12</f>
         <v>15.649452269170579</v>
       </c>
@@ -4785,31 +4791,31 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="24">
+      <c r="J13" s="14">
         <f>AVERAGE(J3:J12)</f>
         <v>15.394079324631225</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="14">
         <f>AVERAGE(K3:K12)</f>
         <v>15.435866592255355</v>
       </c>
-      <c r="L13" s="24">
-        <f t="shared" ref="L13" si="2">AVERAGE(L3:L12)</f>
+      <c r="L13" s="14">
+        <f t="shared" ref="L13" si="7">AVERAGE(L3:L12)</f>
         <v>15.418693647044245</v>
       </c>
-      <c r="W13" s="15"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="22"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4817,20 +4823,20 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="13">
         <f t="array" ref="C15:D16">LINEST(I3:I12,H3:H12,TRUE,TRUE)</f>
         <v>-0.96409120532709625</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="13">
         <v>6.393354451691699E-2</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="32"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
@@ -4838,16 +4844,16 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="13">
         <v>1.6959264966798147E-2</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="13">
         <v>5.9871925775196099E-4</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
@@ -4855,35 +4861,35 @@
       <c r="B17" s="8"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="17"/>
+      <c r="C18" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="22"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="22" t="e">
-        <f t="array" ref="C19:D20">LINEST(I7:I16,H7:H16,TRUE,TRUE)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" s="22" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="32" t="s">
+      <c r="C19" s="13">
+        <f t="array" ref="C19:D20">LINEST(B3:B6,C3:C6,TRUE,TRUE)</f>
+        <v>-16.589928057553816</v>
+      </c>
+      <c r="D19" s="13">
+        <v>410.71654676258731</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="32"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -4898,16 +4904,16 @@
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="22" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D20" s="22" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="33" t="s">
+      <c r="C20" s="13">
+        <v>28.462497469962724</v>
+      </c>
+      <c r="D20" s="13">
+        <v>525.50560050114461</v>
+      </c>
+      <c r="E20" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="33"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -4928,10 +4934,10 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="17"/>
+      <c r="C22" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="22"/>
       <c r="F22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -4941,20 +4947,20 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="22" t="e">
-        <f t="array" ref="C23:D24">LINEST(I11:I20,H11:H20,TRUE,TRUE)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D23" s="22" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E23" s="32" t="s">
+      <c r="C23" s="13">
+        <f t="array" ref="C23:D24">LINEST(B7:B12,C7:C12,TRUE,TRUE)</f>
+        <v>0.96677244236062876</v>
+      </c>
+      <c r="D23" s="13">
+        <v>21.914179102717483</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="32"/>
+      <c r="F23" s="23"/>
       <c r="Y23" s="3">
         <v>0</v>
       </c>
@@ -4963,16 +4969,16 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="22" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D24" s="22" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E24" s="33" t="s">
+      <c r="C24" s="13">
+        <v>6.6510154776783679E-3</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.62669503418386863</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="24"/>
       <c r="Y24" s="3">
         <v>0</v>
       </c>
@@ -4996,19 +5002,19 @@
       <c r="D27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="27"/>
       <c r="Y27" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="20"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="11">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(B7:B12,C7:C12))/(SLOPE(B7:B12,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>22.145526015082648</v>
@@ -5028,77 +5034,77 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="23">
+      <c r="B29" s="29"/>
+      <c r="C29" s="26">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(Y19:Y24,C7:C12))/(SLOPE(Y19:Y24,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="25">
         <f>SLOPE(B3:B6,C3:C6)*C29+INTERCEPT(B3:B6,C3:C6)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="26">
         <f>C29</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="F29" s="23"/>
+      <c r="F29" s="26"/>
       <c r="Y29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
       <c r="Y30" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="12">
+      <c r="B31" s="29"/>
+      <c r="C31" s="25">
         <v>0</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="25">
         <v>21.914000000000001</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="25">
         <f>D31</f>
         <v>21.914000000000001</v>
       </c>
-      <c r="F31" s="12"/>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
@@ -5119,7 +5125,7 @@
       <c r="G35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H35" s="31" t="s">
+      <c r="H35" s="17" t="s">
         <v>31</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -5136,7 +5142,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="9">
@@ -5154,27 +5160,27 @@
       <c r="F36" s="9">
         <v>3.7</v>
       </c>
-      <c r="G36" s="25">
+      <c r="G36" s="15">
         <f>F36/E36</f>
         <v>1.6086956521739133</v>
       </c>
-      <c r="H36" s="25">
+      <c r="H36" s="15">
         <f>1/C36</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I36" s="25">
+      <c r="I36" s="15">
         <f>1/D36</f>
         <v>4.0816326530612242E-2</v>
       </c>
-      <c r="J36" s="25">
+      <c r="J36" s="15">
         <f>D36*C36/B36</f>
         <v>9.3037974683544302</v>
       </c>
-      <c r="K36" s="25">
+      <c r="K36" s="15">
         <f>C36-C36^2/B36</f>
         <v>9.3037974683544302</v>
       </c>
-      <c r="L36" s="25">
+      <c r="L36" s="15">
         <f>D36-D36^2/B36</f>
         <v>9.3037974683544302</v>
       </c>
@@ -5198,28 +5204,28 @@
       <c r="F37" s="9">
         <v>4</v>
       </c>
-      <c r="G37" s="25">
-        <f t="shared" ref="G37:G38" si="3">F37/E37</f>
+      <c r="G37" s="15">
+        <f t="shared" ref="G37:G38" si="8">F37/E37</f>
         <v>1.7391304347826089</v>
       </c>
-      <c r="H37" s="25">
-        <f t="shared" ref="H37:H38" si="4">1/C37</f>
+      <c r="H37" s="15">
+        <f t="shared" ref="H37:H38" si="9">1/C37</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I37" s="25">
-        <f t="shared" ref="I37:I38" si="5">1/D37</f>
+      <c r="I37" s="15">
+        <f t="shared" ref="I37:I38" si="10">1/D37</f>
         <v>3.4602076124567477E-2</v>
       </c>
-      <c r="J37" s="25">
-        <f t="shared" ref="J37:J38" si="6">D37*C37/B37</f>
+      <c r="J37" s="15">
+        <f t="shared" ref="J37:J38" si="11">D37*C37/B37</f>
         <v>9.8747152619589986</v>
       </c>
-      <c r="K37" s="25">
-        <f t="shared" ref="K37:K38" si="7">C37-C37^2/B37</f>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K38" si="12">C37-C37^2/B37</f>
         <v>9.8747152619589968</v>
       </c>
-      <c r="L37" s="25">
-        <f t="shared" ref="L37:L38" si="8">D37-D37^2/B37</f>
+      <c r="L37" s="15">
+        <f t="shared" ref="L37:L38" si="13">D37-D37^2/B37</f>
         <v>9.8747152619589968</v>
       </c>
     </row>
@@ -5242,55 +5248,69 @@
       <c r="F38" s="9">
         <v>4.3</v>
       </c>
-      <c r="G38" s="25">
-        <f t="shared" si="3"/>
+      <c r="G38" s="15">
+        <f t="shared" si="8"/>
         <v>1.8695652173913044</v>
       </c>
-      <c r="H38" s="25">
-        <f t="shared" si="4"/>
+      <c r="H38" s="15">
+        <f t="shared" si="9"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I38" s="25">
-        <f t="shared" si="5"/>
+      <c r="I38" s="15">
+        <f t="shared" si="10"/>
         <v>3.7383177570093455E-2</v>
       </c>
-      <c r="J38" s="25">
-        <f t="shared" si="6"/>
+      <c r="J38" s="15">
+        <f t="shared" si="11"/>
         <v>9.7272727272727266</v>
       </c>
-      <c r="K38" s="25">
-        <f t="shared" si="7"/>
+      <c r="K38" s="15">
+        <f t="shared" si="12"/>
         <v>9.5454545454545467</v>
       </c>
-      <c r="L38" s="25">
-        <f t="shared" si="8"/>
+      <c r="L38" s="15">
+        <f t="shared" si="13"/>
         <v>9.4030303030303024</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="25">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="15">
         <f>AVERAGE(J36:J38)</f>
         <v>9.6352618191953852</v>
       </c>
-      <c r="K39" s="25">
-        <f t="shared" ref="K39:L39" si="9">AVERAGE(K36:K38)</f>
+      <c r="K39" s="15">
+        <f t="shared" ref="K39:L39" si="14">AVERAGE(K36:K38)</f>
         <v>9.5746557585893246</v>
       </c>
-      <c r="L39" s="25">
-        <f t="shared" si="9"/>
+      <c r="L39" s="15">
+        <f t="shared" si="14"/>
         <v>9.5271810111145765</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AA12:AA13"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="E31:F32"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="W10:X11"/>
+    <mergeCell ref="W12:X13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Y12:Y13"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="Z10:Z11"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B34:L34"/>
     <mergeCell ref="C18:D18"/>
@@ -5299,26 +5319,12 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="AA12:AA13"/>
-    <mergeCell ref="E29:F30"/>
-    <mergeCell ref="E31:F32"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="A31:B32"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="D31:D32"/>
-    <mergeCell ref="W10:X11"/>
-    <mergeCell ref="W12:X13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B30"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Y12:Y13"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="Z10:Z11"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
   </mergeCells>
@@ -5335,6 +5341,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A6AC9AE00E36404AA0D09428E6D89785" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="90a733a5ab80369601faf008bc080d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c5de1c3e-7813-4da7-ba52-5366b85aaf02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b20cf44b89237f95aaad323f9088c9f4" ns3:_="">
     <xsd:import namespace="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
@@ -5480,15 +5495,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
   <ds:schemaRefs>
@@ -5506,6 +5512,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE32EF5C-8F83-4888-B6EF-0E9A1DA73572}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5521,12 +5535,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
T7A - 2 tabelas de análise estatística apagadas
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCE4159-77F4-41E4-A524-67E8503BBA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC78E3A-FFA4-48D7-8D15-1C67F6F77241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>D (cm)</t>
   </si>
@@ -134,12 +134,6 @@
   </si>
   <si>
     <t>1/Si (cm-1)</t>
-  </si>
-  <si>
-    <t>Reta da Esquerda</t>
-  </si>
-  <si>
-    <t>Reta da Direita</t>
   </si>
 </sst>
 </file>
@@ -346,6 +340,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,35 +379,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4227,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34871357-AA4E-4AD0-9D7D-AF7CAC853938}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4249,19 +4243,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -4659,17 +4653,17 @@
         <f t="shared" si="4"/>
         <v>16.005086245024327</v>
       </c>
-      <c r="W10" s="28" t="s">
+      <c r="W10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="25">
+      <c r="X10" s="22"/>
+      <c r="Y10" s="18">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="Z10" s="25">
+      <c r="Z10" s="18">
         <v>0</v>
       </c>
-      <c r="AA10" s="25">
+      <c r="AA10" s="18">
         <f>1/ Y10</f>
         <v>15.105740181268883</v>
       </c>
@@ -4717,11 +4711,11 @@
         <f t="shared" si="4"/>
         <v>15.499778761061947</v>
       </c>
-      <c r="W11" s="28"/>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -4766,17 +4760,17 @@
         <f t="shared" si="4"/>
         <v>15.271057655593737</v>
       </c>
-      <c r="W12" s="28" t="s">
+      <c r="W12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="25">
+      <c r="X12" s="22"/>
+      <c r="Y12" s="18">
         <v>0</v>
       </c>
-      <c r="Z12" s="25">
+      <c r="Z12" s="18">
         <v>6.3899999999999998E-2</v>
       </c>
-      <c r="AA12" s="25">
+      <c r="AA12" s="18">
         <f>1/Z12</f>
         <v>15.649452269170579</v>
       </c>
@@ -4803,19 +4797,19 @@
         <f t="shared" ref="L13" si="7">AVERAGE(L3:L12)</f>
         <v>15.418693647044245</v>
       </c>
-      <c r="W13" s="28"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="30"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4861,35 +4855,13 @@
       <c r="B17" s="8"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="F18" s="3"/>
-    </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="13">
-        <f t="array" ref="C19:D20">LINEST(B3:B6,C3:C6,TRUE,TRUE)</f>
-        <v>-16.589928057553816</v>
-      </c>
-      <c r="D19" s="13">
-        <v>410.71654676258731</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="23"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -4901,19 +4873,6 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="13">
-        <v>28.462497469962724</v>
-      </c>
-      <c r="D20" s="13">
-        <v>525.50560050114461</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="24"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -4933,12 +4892,6 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="F22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -4947,38 +4900,11 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B23" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="13">
-        <f t="array" ref="C23:D24">LINEST(B7:B12,C7:C12,TRUE,TRUE)</f>
-        <v>0.96677244236062876</v>
-      </c>
-      <c r="D23" s="13">
-        <v>21.914179102717483</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="23"/>
       <c r="Y23" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="13">
-        <v>6.6510154776783679E-3</v>
-      </c>
-      <c r="D24" s="13">
-        <v>0.62669503418386863</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="24"/>
       <c r="Y24" s="3">
         <v>0</v>
       </c>
@@ -5002,16 +4928,16 @@
       <c r="D27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="20"/>
       <c r="Y27" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="33"/>
@@ -5034,77 +4960,77 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="26">
+      <c r="B29" s="31"/>
+      <c r="C29" s="19">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(Y19:Y24,C7:C12))/(SLOPE(Y19:Y24,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="18">
         <f>SLOPE(B3:B6,C3:C6)*C29+INTERCEPT(B3:B6,C3:C6)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="19">
         <f>C29</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="F29" s="26"/>
+      <c r="F29" s="19"/>
       <c r="Y29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
       <c r="Y30" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="25">
+      <c r="B31" s="31"/>
+      <c r="C31" s="18">
         <v>0</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="18">
         <v>21.914000000000001</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="18">
         <f>D31</f>
         <v>21.914000000000001</v>
       </c>
-      <c r="F31" s="25"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
@@ -5296,7 +5222,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="24">
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="AA10:AA11"/>
     <mergeCell ref="AA12:AA13"/>
     <mergeCell ref="E29:F30"/>
@@ -5311,22 +5247,6 @@
     <mergeCell ref="Y12:Y13"/>
     <mergeCell ref="Z12:Z13"/>
     <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
   </mergeCells>
   <pageMargins left="0.01" right="0.01" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5341,15 +5261,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A6AC9AE00E36404AA0D09428E6D89785" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="90a733a5ab80369601faf008bc080d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c5de1c3e-7813-4da7-ba52-5366b85aaf02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b20cf44b89237f95aaad323f9088c9f4" ns3:_="">
     <xsd:import namespace="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
@@ -5495,6 +5406,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
   <ds:schemaRefs>
@@ -5512,14 +5432,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE32EF5C-8F83-4888-B6EF-0E9A1DA73572}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5535,4 +5447,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
T7A - versão 100% final
- resíduos corrigidos
- legendas dos gráficos com fronteira a preto
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive - Universidade do Porto\Ambiente de Trabalho\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8130D7-459C-4E03-B78F-F35F7788DA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1FC5B-A206-4EF2-B74F-1E846F99BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -492,12 +492,6 @@
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,60 +505,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -588,7 +528,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -611,7 +605,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -678,7 +672,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -799,7 +793,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -990,7 +984,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1028,7 +1022,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="562182383"/>
@@ -1117,7 +1111,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1155,7 +1149,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="744089615"/>
@@ -1176,10 +1170,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12087471244526332"/>
-          <c:y val="0.72543554325165616"/>
-          <c:w val="0.20390317023592699"/>
-          <c:h val="0.20629955457522206"/>
+          <c:x val="0.14042397295924999"/>
+          <c:y val="0.74149114403890992"/>
+          <c:w val="0.22345232233837131"/>
+          <c:h val="7.3841658114801173E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1207,7 +1201,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1228,10 +1222,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1244,7 +1235,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1258,7 +1249,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1328,7 +1319,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1435,7 +1426,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1580,7 +1571,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1729,7 +1720,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1767,7 +1758,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="414115519"/>
@@ -1859,7 +1850,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1897,7 +1888,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="414116351"/>
@@ -1926,17 +1917,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65700667444689009"/>
-          <c:y val="0.46353000874890637"/>
-          <c:w val="0.26761645770047582"/>
+          <c:x val="0.67644998450442484"/>
+          <c:y val="0.45901151744837215"/>
+          <c:w val="0.2537285065874238"/>
           <c:h val="0.34000629921259845"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1957,7 +1952,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1978,10 +1973,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1994,7 +1986,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2008,7 +2000,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2078,7 +2070,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2128,39 +2120,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$32:$G$41</c:f>
+              <c:f>Sheet1!$H$3:$H$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.1503260869565213E-2</c:v>
+                  <c:v>5.4347826086956527E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2343850267379684E-2</c:v>
+                  <c:v>5.3475935828877004E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1645257452574526E-2</c:v>
+                  <c:v>5.4200542005420058E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1216939890710383E-2</c:v>
+                  <c:v>5.4644808743169397E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1313838120104441E-2</c:v>
+                  <c:v>1.3054830287206267E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.226330718165359E-2</c:v>
+                  <c:v>1.2070006035003019E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2931854379977245E-2</c:v>
+                  <c:v>1.1376564277588168E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3643617021276596E-2</c:v>
+                  <c:v>1.0638297872340425E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.481328934967012E-2</c:v>
+                  <c:v>9.4250706880301613E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5351498492640538E-2</c:v>
+                  <c:v>8.8668203582195418E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8210070218281064E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2226,6 +2221,7 @@
         <c:axId val="2028769919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2310,11 +2306,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2348,7 +2344,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2028775327"/>
@@ -2437,7 +2433,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2475,7 +2471,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2028769919"/>
@@ -2496,17 +2492,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17575460678365018"/>
-          <c:y val="0.77596023718630835"/>
+          <c:x val="0.19510125062783834"/>
+          <c:y val="0.74846225048221016"/>
           <c:w val="0.13489348206474192"/>
           <c:h val="7.8125546806649182E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -2527,7 +2527,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2548,10 +2548,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2564,7 +2561,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2578,7 +2575,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2640,7 +2637,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2667,7 +2664,7 @@
             <c:v>Resíduos</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2690,54 +2687,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$32:$H$37</c:f>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>74.120779999999996</c:v>
+                  <c:v>18.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.16328</c:v>
+                  <c:v>18.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.045620000000014</c:v>
+                  <c:v>18.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.943100000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>102.64138</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>109.099604</c:v>
+                  <c:v>18.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$32:$K$37</c:f>
+              <c:f>Sheet1!$L$38:$L$41</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-0.22087999999999397</c:v>
+                  <c:v>-9.8640000000000612</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13662000000000774</c:v>
+                  <c:v>1.6129999999999711</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2799999999942884E-3</c:v>
+                  <c:v>2.2654999999999461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25679999999999836</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.19147999999999854</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9599999999163629E-4</c:v>
+                  <c:v>5.9770000000000039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2764,8 +2749,8 @@
         <c:axId val="1663020895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="115"/>
-          <c:min val="68"/>
+          <c:max val="18.8"/>
+          <c:min val="18.2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2834,11 +2819,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2872,7 +2857,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1663015487"/>
@@ -2959,11 +2944,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2997,7 +2982,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1663020895"/>
@@ -3018,17 +3003,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79452148071861117"/>
-          <c:y val="0.20166320608336952"/>
-          <c:w val="0.14919094790570533"/>
+          <c:x val="0.7784081753759593"/>
+          <c:y val="0.20699941933407451"/>
+          <c:w val="0.13307751298541112"/>
           <c:h val="8.7719894251836669E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -3049,7 +3038,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3070,10 +3059,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -3086,7 +3072,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3100,7 +3086,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3175,42 +3161,54 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$38:$I$41</c:f>
+              <c:f>Sheet1!$C$7:$C$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>105.46400000000006</c:v>
+                  <c:v>76.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.48700000000002</c:v>
+                  <c:v>82.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104.63450000000006</c:v>
+                  <c:v>87.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107.12299999999999</c:v>
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$38:$L$41</c:f>
+              <c:f>Sheet1!$K$32:$K$37</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-9.8640000000000612</c:v>
+                  <c:v>-0.22087999999999397</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6129999999999711</c:v>
+                  <c:v>0.13662000000000774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2654999999999461</c:v>
+                  <c:v>4.2799999999942884E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9770000000000039</c:v>
+                  <c:v>0.25679999999999836</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.19147999999999854</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9599999999163629E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3329,8 +3327,8 @@
         <c:axId val="1663020895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="108"/>
-          <c:min val="98"/>
+          <c:max val="120"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3396,7 +3394,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3430,7 +3428,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1663015487"/>
@@ -3441,7 +3439,8 @@
         <c:axId val="1663015487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-11"/>
+          <c:max val="0.5"/>
+          <c:min val="-0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3502,7 +3501,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3536,7 +3535,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1663020895"/>
@@ -3550,17 +3549,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15524754870004101"/>
-          <c:y val="0.68135108437052705"/>
-          <c:w val="0.16858079806998721"/>
-          <c:h val="0.17475846907556117"/>
+          <c:x val="0.81703884140323202"/>
+          <c:y val="0.21833327058842178"/>
+          <c:w val="0.1201569895425036"/>
+          <c:h val="0.10429908319777133"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -3581,7 +3584,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3590,6 +3593,13 @@
     <c:showDLblsOverMax val="0"/>
     <c:extLst/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -3597,7 +3607,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5837,15 +5847,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>48619</xdr:rowOff>
+      <xdr:colOff>432706</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>135703</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>88444</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5873,15 +5883,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>118109</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>109930</xdr:rowOff>
+      <xdr:colOff>433794</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>186129</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>3250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>96610</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>144764</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6215,15 +6225,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>439510</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>65995</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>125185</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>61233</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6250,15 +6260,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>64771</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>238942</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>120967</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>520066</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>84637</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6288,16 +6298,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>70485</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>277314</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>108177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>516255</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>113484</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>84365</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6328,7 +6338,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6624,10 +6634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34871357-AA4E-4AD0-9D7D-AF7CAC853938}">
-  <dimension ref="A1:AC42"/>
+  <dimension ref="A1:AC45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6649,19 +6659,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -7189,25 +7199,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="56"/>
       <c r="E15" s="3"/>
-      <c r="G15" s="48" t="s">
+      <c r="G15" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="48"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="48"/>
+      <c r="L15" s="49"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
@@ -7220,14 +7230,14 @@
       <c r="C16" s="11">
         <v>6.393354451691699E-2</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="G16" s="45" t="s">
+      <c r="E16" s="46"/>
+      <c r="G16" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="46"/>
+      <c r="H16" s="58"/>
       <c r="I16" s="10">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(B7:B12,C7:C12))/(SLOPE(B7:B12,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>22.145526015082648</v>
@@ -7253,73 +7263,73 @@
       <c r="C17" s="11">
         <v>5.9871925775196099E-4</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="53"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="47">
+      <c r="H17" s="54"/>
+      <c r="I17" s="59">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(R24:R29,C7:C12))/(SLOPE(R24:R29,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="J17" s="43">
+      <c r="J17" s="41">
         <f>SLOPE(B3:B6,C3:C6)*I17+INTERCEPT(B3:B6,C3:C6)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="59">
         <f>I17</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="L17" s="47"/>
+      <c r="L17" s="59"/>
     </row>
     <row r="18" spans="1:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="42"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="G19" s="40" t="s">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="G19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="43">
+      <c r="H19" s="54"/>
+      <c r="I19" s="41">
         <v>0</v>
       </c>
-      <c r="J19" s="43">
+      <c r="J19" s="41">
         <v>21.914000000000001</v>
       </c>
-      <c r="K19" s="43">
+      <c r="K19" s="41">
         <f>J19</f>
         <v>21.914000000000001</v>
       </c>
-      <c r="L19" s="43"/>
+      <c r="L19" s="41"/>
     </row>
     <row r="20" spans="1:29" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="60"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B21" s="22"/>
@@ -7330,23 +7340,23 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A22" s="58"/>
-      <c r="B22" s="39" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" s="59"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="17" t="s">
         <v>0</v>
       </c>
@@ -7572,10 +7582,10 @@
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="48"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
@@ -7585,96 +7595,64 @@
       <c r="E29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="61" t="s">
+      <c r="G29" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61" t="s">
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
       <c r="R29" s="3">
         <v>0</v>
       </c>
-      <c r="Y29" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z29" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB29" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC29" s="18" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="49"/>
-      <c r="C30" s="43">
+      <c r="B30" s="44"/>
+      <c r="C30" s="41">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="D30" s="43">
+      <c r="D30" s="41">
         <v>0</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="41">
         <f>1/ C30</f>
         <v>15.105740181268883</v>
       </c>
       <c r="G30" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="61" t="s">
+      <c r="H30" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="61"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K30" s="61" t="s">
+      <c r="K30" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="L30" s="61"/>
+      <c r="L30" s="42"/>
       <c r="R30" s="3">
         <v>0</v>
       </c>
-      <c r="Y30" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z30" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA30" s="31">
-        <f>J13</f>
-        <v>15.394079324631225</v>
-      </c>
-      <c r="AB30" s="32">
-        <v>0.378</v>
-      </c>
-      <c r="AC30" s="33">
-        <f>((AA30-15)/15)</f>
-        <v>2.6271954975414975E-2</v>
-      </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
       <c r="G31" s="1"/>
       <c r="H31" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="I31" s="24" t="s">
         <v>43</v>
       </c>
       <c r="J31" s="1"/>
@@ -7687,34 +7665,19 @@
       <c r="R31" s="3">
         <v>0</v>
       </c>
-      <c r="Y31" s="54"/>
-      <c r="Z31" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA31" s="31">
-        <f>K13</f>
-        <v>15.435866592255355</v>
-      </c>
-      <c r="AB31" s="32">
-        <v>0.94199999999999995</v>
-      </c>
-      <c r="AC31" s="33">
-        <f t="shared" ref="AC31:AC36" si="16">((AA31-15)/15)</f>
-        <v>2.9057772817023656E-2</v>
-      </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="43">
+      <c r="B32" s="44"/>
+      <c r="C32" s="41">
         <v>0</v>
       </c>
-      <c r="D32" s="43">
+      <c r="D32" s="41">
         <v>6.3899999999999998E-2</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="41">
         <f>1/D32</f>
         <v>15.649452269170579</v>
       </c>
@@ -7739,28 +7702,28 @@
       <c r="R32" s="3">
         <v>0</v>
       </c>
-      <c r="Y32" s="54"/>
-      <c r="Z32" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA32" s="31">
-        <f>L13</f>
-        <v>15.418693647044245</v>
-      </c>
-      <c r="AB32" s="32">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="AC32" s="33">
-        <f t="shared" si="16"/>
-        <v>2.7912909802949672E-2</v>
+      <c r="Y32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA32" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB32" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC32" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
       <c r="G33" s="27">
         <v>1.2343850267379684E-2</v>
       </c>
@@ -7778,19 +7741,22 @@
       <c r="R33" s="3">
         <v>0</v>
       </c>
-      <c r="Y33" s="54"/>
-      <c r="Z33" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA33" s="32">
-        <v>-0.96409999999999996</v>
-      </c>
-      <c r="AB33" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC33" s="33">
-        <f>((AA33+1)/(-1))</f>
-        <v>-3.5900000000000043E-2</v>
+      <c r="Y33" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z33" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA33" s="29">
+        <f>J13</f>
+        <v>15.394079324631225</v>
+      </c>
+      <c r="AB33" s="30">
+        <v>0.378</v>
+      </c>
+      <c r="AC33" s="31">
+        <f>((AA33-15)/15)</f>
+        <v>2.6271954975414975E-2</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
@@ -7811,20 +7777,20 @@
       <c r="R34" s="3">
         <v>0</v>
       </c>
-      <c r="Y34" s="54"/>
-      <c r="Z34" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA34" s="32">
-        <f>E32</f>
-        <v>15.649452269170579</v>
-      </c>
-      <c r="AB34" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC34" s="33">
-        <f t="shared" si="16"/>
-        <v>4.3296817944705288E-2</v>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA34" s="29">
+        <f>K13</f>
+        <v>15.435866592255355</v>
+      </c>
+      <c r="AB34" s="30">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="AC34" s="31">
+        <f t="shared" ref="AC34:AC39" si="16">((AA34-15)/15)</f>
+        <v>2.9057772817023656E-2</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
@@ -7845,20 +7811,20 @@
       <c r="R35" s="3">
         <v>0</v>
       </c>
-      <c r="Y35" s="54"/>
-      <c r="Z35" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA35" s="32">
-        <f>E30</f>
-        <v>15.105740181268883</v>
-      </c>
-      <c r="AB35" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC35" s="33">
+      <c r="Y35" s="36"/>
+      <c r="Z35" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA35" s="29">
+        <f>L13</f>
+        <v>15.418693647044245</v>
+      </c>
+      <c r="AB35" s="30">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="AC35" s="31">
         <f t="shared" si="16"/>
-        <v>7.0493454179255599E-3</v>
+        <v>2.7912909802949672E-2</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
@@ -7876,20 +7842,19 @@
         <v>-0.19147999999999854</v>
       </c>
       <c r="L36" s="25"/>
-      <c r="Y36" s="54"/>
-      <c r="Z36" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA36" s="32">
-        <f>K16</f>
-        <v>11.073</v>
-      </c>
-      <c r="AB36" s="34" t="s">
+      <c r="Y36" s="36"/>
+      <c r="Z36" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA36" s="30">
+        <v>-0.96409999999999996</v>
+      </c>
+      <c r="AB36" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AC36" s="33">
-        <f t="shared" si="16"/>
-        <v>-0.26179999999999998</v>
+      <c r="AC36" s="31">
+        <f>((AA36+1)/(-1))</f>
+        <v>-3.5900000000000043E-2</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
@@ -7907,20 +7872,20 @@
         <v>2.9599999999163629E-4</v>
       </c>
       <c r="L37" s="25"/>
-      <c r="Y37" s="54"/>
-      <c r="Z37" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA37" s="32">
-        <f>L16</f>
-        <v>10.831</v>
-      </c>
-      <c r="AB37" s="34" t="s">
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA37" s="30">
+        <f>E32</f>
+        <v>15.649452269170579</v>
+      </c>
+      <c r="AB37" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AC37" s="33">
-        <f>((AA37-15)/15)</f>
-        <v>-0.27793333333333337</v>
+      <c r="AC37" s="31">
+        <f t="shared" si="16"/>
+        <v>4.3296817944705288E-2</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
@@ -7940,20 +7905,20 @@
         <f t="array" ref="L38:L41">(B3:B6)-(-16.59*C3:C6+410.72)</f>
         <v>-9.8640000000000612</v>
       </c>
-      <c r="Y38" s="54"/>
-      <c r="Z38" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA38" s="32">
-        <f>K19</f>
-        <v>21.914000000000001</v>
-      </c>
-      <c r="AB38" s="34" t="s">
+      <c r="Y38" s="36"/>
+      <c r="Z38" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA38" s="30">
+        <f>E30</f>
+        <v>15.105740181268883</v>
+      </c>
+      <c r="AB38" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AC38" s="33">
-        <f>((AA38-15)/15)</f>
-        <v>0.46093333333333342</v>
+      <c r="AC38" s="31">
+        <f t="shared" si="16"/>
+        <v>7.0493454179255599E-3</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
@@ -7971,20 +7936,20 @@
       <c r="L39" s="20">
         <v>1.6129999999999711</v>
       </c>
-      <c r="Y39" s="54"/>
-      <c r="Z39" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA39" s="35">
-        <f>K17</f>
-        <v>24.756981786643593</v>
-      </c>
-      <c r="AB39" s="34" t="s">
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA39" s="30">
+        <f>K16</f>
+        <v>11.073</v>
+      </c>
+      <c r="AB39" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AC39" s="33">
-        <f>((AA39-15)/15)</f>
-        <v>0.65046545244290621</v>
+      <c r="AC39" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.26179999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
@@ -8002,22 +7967,20 @@
       <c r="L40" s="20">
         <v>2.2654999999999461</v>
       </c>
-      <c r="Y40" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z40" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA40" s="31">
-        <f>J27</f>
-        <v>9.6352618191953852</v>
-      </c>
-      <c r="AB40" s="32">
-        <v>3.9E-2</v>
-      </c>
-      <c r="AC40" s="33">
-        <f>((AA40-10)/10)</f>
-        <v>-3.6473818080461483E-2</v>
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA40" s="30">
+        <f>L16</f>
+        <v>10.831</v>
+      </c>
+      <c r="AB40" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC40" s="31">
+        <f>((AA40-15)/15)</f>
+        <v>-0.27793333333333337</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
@@ -8035,60 +7998,94 @@
       <c r="L41" s="20">
         <v>5.9770000000000039</v>
       </c>
-      <c r="Y41" s="56"/>
-      <c r="Z41" s="29" t="s">
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA41" s="30">
+        <f>K19</f>
+        <v>21.914000000000001</v>
+      </c>
+      <c r="AB41" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC41" s="31">
+        <f>((AA41-15)/15)</f>
+        <v>0.46093333333333342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y42" s="37"/>
+      <c r="Z42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA42" s="33">
+        <f>K17</f>
+        <v>24.756981786643593</v>
+      </c>
+      <c r="AB42" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC42" s="31">
+        <f>((AA42-15)/15)</f>
+        <v>0.65046545244290621</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y43" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z43" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA43" s="29">
+        <f>J27</f>
+        <v>9.6352618191953852</v>
+      </c>
+      <c r="AB43" s="30">
+        <v>3.9E-2</v>
+      </c>
+      <c r="AC43" s="31">
+        <f>((AA43-10)/10)</f>
+        <v>-3.6473818080461483E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y44" s="36"/>
+      <c r="Z44" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="AA41" s="31">
+      <c r="AA44" s="29">
         <f>K27</f>
         <v>9.5746557585893246</v>
       </c>
-      <c r="AB41" s="32">
+      <c r="AB44" s="30">
         <v>0.96399999999999997</v>
       </c>
-      <c r="AC41" s="33">
-        <f t="shared" ref="AC41:AC42" si="17">((AA41-10)/10)</f>
+      <c r="AC44" s="31">
+        <f t="shared" ref="AC44:AC45" si="17">((AA44-10)/10)</f>
         <v>-4.2534424141067541E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Y42" s="57"/>
-      <c r="Z42" s="29" t="s">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AA42" s="31">
+      <c r="AA45" s="29">
         <f>L27</f>
         <v>9.5271810111145765</v>
       </c>
-      <c r="AB42" s="32">
+      <c r="AB45" s="30">
         <v>0.93600000000000005</v>
       </c>
-      <c r="AC42" s="33">
+      <c r="AC45" s="31">
         <f t="shared" si="17"/>
         <v>-4.7281898888542354E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="Y30:Y39"/>
-    <mergeCell ref="Y40:Y42"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A19:E20"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A29:B29"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B22:L22"/>
     <mergeCell ref="G19:H20"/>
@@ -8103,6 +8100,25 @@
     <mergeCell ref="K19:L20"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="Y33:Y42"/>
+    <mergeCell ref="Y43:Y45"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A19:E20"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="3.937007874015748E-2" footer="3.937007874015748E-2"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8111,21 +8127,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A6AC9AE00E36404AA0D09428E6D89785" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="90a733a5ab80369601faf008bc080d09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c5de1c3e-7813-4da7-ba52-5366b85aaf02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b20cf44b89237f95aaad323f9088c9f4" ns3:_="">
     <xsd:import namespace="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
@@ -8271,31 +8272,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE32EF5C-8F83-4888-B6EF-0E9A1DA73572}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8311,4 +8303,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D33A98F-BD38-4038-820D-29FB47F72D1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7DCA3E-FE35-4BAD-8434-94F53402176D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
t7A - mesmo final
- erros percentuais positivos
- So e SO corrigido
</commit_message>
<xml_diff>
--- a/T7A - lentes.xlsx
+++ b/T7A - lentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1FC5B-A206-4EF2-B74F-1E846F99BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011CB4F7-5F7E-4866-92B8-82FDDC33B0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86E8DEF9-3212-4254-81AD-B9280C6CFF3C}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
   <si>
     <t>D (cm)</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>In.Assintotas (Y/4) (2)</t>
+  </si>
+  <si>
+    <t>1/So</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,18 +543,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,6 +574,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -641,7 +647,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> de 1/S0</a:t>
+              <a:t> de 1/So</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1289,7 +1295,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>S0</a:t>
+              <a:t>So</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1690,7 +1696,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1300"/>
-                  <a:t>S0 (cm)</a:t>
+                  <a:t>So (cm)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6636,8 +6642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34871357-AA4E-4AD0-9D7D-AF7CAC853938}">
   <dimension ref="A1:AC45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X40" sqref="X40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6659,19 +6665,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="52"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -6694,7 +6700,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>8</v>
@@ -7199,25 +7205,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="56"/>
+      <c r="C15" s="52"/>
       <c r="E15" s="3"/>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="49"/>
+      <c r="H15" s="45"/>
       <c r="I15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="49" t="s">
+      <c r="K15" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="49"/>
+      <c r="L15" s="45"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
@@ -7230,14 +7236,14 @@
       <c r="C16" s="11">
         <v>6.393354451691699E-2</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="G16" s="57" t="s">
+      <c r="E16" s="57"/>
+      <c r="G16" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="58"/>
+      <c r="H16" s="54"/>
       <c r="I16" s="10">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(B7:B12,C7:C12))/(SLOPE(B7:B12,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>22.145526015082648</v>
@@ -7263,16 +7269,16 @@
       <c r="C17" s="11">
         <v>5.9871925775196099E-4</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="21"/>
       <c r="G17" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="59">
+      <c r="H17" s="50"/>
+      <c r="I17" s="55">
         <f>(INTERCEPT(B3:B6,C3:C6)-INTERCEPT(R24:R29,C7:C12))/(SLOPE(R24:R29,C7:C12)-SLOPE(B3:B6,C3:C6))</f>
         <v>24.756981786643593</v>
       </c>
@@ -7280,19 +7286,19 @@
         <f>SLOPE(B3:B6,C3:C6)*I17+INTERCEPT(B3:B6,C3:C6)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="59">
+      <c r="K17" s="55">
         <f>I17</f>
         <v>24.756981786643593</v>
       </c>
-      <c r="L17" s="59"/>
+      <c r="L17" s="55"/>
     </row>
     <row r="18" spans="1:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="55"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="59"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="41"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
@@ -7305,7 +7311,7 @@
       <c r="G19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="54"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="41">
         <v>0</v>
       </c>
@@ -7324,8 +7330,8 @@
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="54"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="41"/>
       <c r="J20" s="41"/>
       <c r="K20" s="41"/>
@@ -7341,19 +7347,19 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="38"/>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
@@ -7582,10 +7588,10 @@
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="49"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
@@ -7789,7 +7795,7 @@
         <v>0.94199999999999995</v>
       </c>
       <c r="AC34" s="31">
-        <f t="shared" ref="AC34:AC39" si="16">((AA34-15)/15)</f>
+        <f t="shared" ref="AC34:AC38" si="16">((AA34-15)/15)</f>
         <v>2.9057772817023656E-2</v>
       </c>
     </row>
@@ -7853,8 +7859,8 @@
         <v>30</v>
       </c>
       <c r="AC36" s="31">
-        <f>((AA36+1)/(-1))</f>
-        <v>-3.5900000000000043E-2</v>
+        <f>(ABS(AA36+1)/(1))</f>
+        <v>3.5900000000000043E-2</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
@@ -7937,7 +7943,7 @@
         <v>1.6129999999999711</v>
       </c>
       <c r="Y39" s="36"/>
-      <c r="Z39" s="34" t="s">
+      <c r="Z39" s="60" t="s">
         <v>53</v>
       </c>
       <c r="AA39" s="30">
@@ -7948,8 +7954,8 @@
         <v>30</v>
       </c>
       <c r="AC39" s="31">
-        <f t="shared" si="16"/>
-        <v>-0.26179999999999998</v>
+        <f>(ABS(AA39-15)/15)</f>
+        <v>0.26179999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
@@ -7968,7 +7974,7 @@
         <v>2.2654999999999461</v>
       </c>
       <c r="Y40" s="36"/>
-      <c r="Z40" s="34" t="s">
+      <c r="Z40" s="60" t="s">
         <v>54</v>
       </c>
       <c r="AA40" s="30">
@@ -7979,8 +7985,8 @@
         <v>30</v>
       </c>
       <c r="AC40" s="31">
-        <f>((AA40-15)/15)</f>
-        <v>-0.27793333333333337</v>
+        <f>(ABS(AA40-15)/15)</f>
+        <v>0.27793333333333337</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
@@ -8046,8 +8052,8 @@
         <v>3.9E-2</v>
       </c>
       <c r="AC43" s="31">
-        <f>((AA43-10)/10)</f>
-        <v>-3.6473818080461483E-2</v>
+        <f>(ABS(AA43-10)/10)</f>
+        <v>3.6473818080461483E-2</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.3">
@@ -8063,8 +8069,8 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AC44" s="31">
-        <f t="shared" ref="AC44:AC45" si="17">((AA44-10)/10)</f>
-        <v>-4.2534424141067541E-2</v>
+        <f>(ABS(AA44-10)/10)</f>
+        <v>4.2534424141067541E-2</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.3">
@@ -8080,12 +8086,14 @@
         <v>0.93600000000000005</v>
       </c>
       <c r="AC45" s="31">
-        <f t="shared" si="17"/>
-        <v>-4.7281898888542354E-2</v>
+        <f>(ABS(AA45-10)/10)</f>
+        <v>4.7281898888542354E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="Y33:Y42"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B22:L22"/>
     <mergeCell ref="G19:H20"/>
@@ -8101,12 +8109,6 @@
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="Y33:Y42"/>
     <mergeCell ref="Y43:Y45"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A19:E20"/>
@@ -8119,6 +8121,10 @@
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="3.937007874015748E-2" footer="3.937007874015748E-2"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>